<commit_message>
Subtract slack from total costs in output
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Efficiency_Electrolyzers.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Efficiency_Electrolyzers.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\methanol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9A7EF3-3C5A-4FC5-9102-093E5F530029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{5B9A7EF3-3C5A-4FC5-9102-093E5F530029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7F7EF84-13EB-4175-8230-FCE2B3C6BE57}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3840" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency_PEM" sheetId="5" r:id="rId1"/>
-    <sheet name="Efficiency_Alkaline" sheetId="6" r:id="rId2"/>
-    <sheet name="Efficiency_SOEC" sheetId="7" r:id="rId3"/>
-    <sheet name="Sources" sheetId="2" r:id="rId4"/>
+    <sheet name="Efficiency_PEM2" sheetId="8" r:id="rId2"/>
+    <sheet name="Efficiency_Alkaline" sheetId="6" r:id="rId3"/>
+    <sheet name="Efficiency_SOEC" sheetId="7" r:id="rId4"/>
+    <sheet name="Sources" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="CIQWBGuid" hidden="1">"9dba8f33-1087-4509-8f71-f29d917cc8e9"</definedName>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Power [%]</t>
   </si>
@@ -603,12 +604,13 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -966,10 +968,606 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2433A841-7153-44ED-9730-8ADB27239D68}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:F98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.61993799999999999</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>5.1989999999999996E-3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.62460419999999983</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1.2796999999999999E-2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.62893710000000003</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2.0596E-2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.63360329999999998</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2.8194E-2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.63760289999999997</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>3.5992999999999997E-2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.64193579999999995</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>4.879E-2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.64626869999999992</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>6.4186999999999994E-2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.6506016</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>8.3382999999999999E-2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.65460119999999999</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>0.103979</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.65726759999999995</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0.130774</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.65926739999999995</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>0.15396899999999999</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.65926739999999995</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>0.18216399999999999</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.65893409999999997</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>0.21035799999999999</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.65760090000000004</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>0.244951</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.65560109999999994</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>0.278144</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.65260139999999989</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>0.314137</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.64960169999999995</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>0.34233200000000003</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.64660200000000001</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>0.37832399999999999</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.64326899999999998</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0.408918</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.63993599999999995</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0.441112</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.63660300000000003</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>0.47190599999999999</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.63360329999999998</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>0.50009999999999999</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.63060360000000004</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>0.530694</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.62760389999999999</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>0.56548699999999996</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.62393759999999998</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>0.60647899999999999</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.61993799999999999</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>0.64866999999999997</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.61560509999999991</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>0.689662</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.61193879999999989</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>0.73725300000000005</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.60727259999999994</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>0.78724300000000003</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.60260639999999988</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>0.83583300000000005</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.59860679999999999</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>0.88082400000000005</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.59460719999999989</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>0.92561499999999997</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.59094089999999999</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>0.96020799999999995</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.58760789999999996</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.5849415</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="2"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B38" s="1"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B39" s="1"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B40" s="1"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B41" s="1"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="1"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B43" s="1"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B44" s="1"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B45" s="1"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="1"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B47" s="1"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B48" s="1"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B49" s="1"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B50" s="1"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B51" s="1"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B52" s="1"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B53" s="1"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B54" s="1"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B55" s="1"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B98" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F719D7A-A6A7-44A6-8E8F-0D3A6EF426CF}">
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B36"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,486 +1582,447 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.61993799999999999</v>
+        <v>2.2403258655804437E-2</v>
+      </c>
+      <c r="B2">
+        <v>0.93457943925234699</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>5.1989999999999996E-3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.62460419999999983</v>
+        <v>2.4439918533604787E-2</v>
+      </c>
+      <c r="B3">
+        <v>3.73831775700934</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>1.2796999999999999E-2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.62893710000000003</v>
+        <v>2.6476578411405282E-2</v>
+      </c>
+      <c r="B4">
+        <v>7.4766355140186898</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>2.0596E-2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.63360329999999998</v>
+        <v>2.6476578411405282E-2</v>
+      </c>
+      <c r="B5">
+        <v>10.9034267912772</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>2.8194E-2</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.63760289999999997</v>
+        <v>2.6476578411405282E-2</v>
+      </c>
+      <c r="B6">
+        <v>13.0841121495327</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>3.5992999999999997E-2</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.64193579999999995</v>
+        <v>3.0549898167005984E-2</v>
+      </c>
+      <c r="B7">
+        <v>15.887850467289699</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>4.879E-2</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.64626869999999992</v>
+        <v>3.258655804480648E-2</v>
+      </c>
+      <c r="B8">
+        <v>18.068535825545101</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>6.4186999999999994E-2</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.6506016</v>
+        <v>3.4623217922606829E-2</v>
+      </c>
+      <c r="B9">
+        <v>20.5607476635514</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>8.3382999999999999E-2</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.65460119999999999</v>
+        <v>3.6659877800407324E-2</v>
+      </c>
+      <c r="B10">
+        <v>24.299065420560702</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>0.103979</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.65726759999999995</v>
+        <v>3.8696537678207674E-2</v>
+      </c>
+      <c r="B11">
+        <v>28.037383177570103</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>0.130774</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.65926739999999995</v>
+        <v>4.073319755600803E-2</v>
+      </c>
+      <c r="B12">
+        <v>31.464174454828598</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>0.15396899999999999</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.65926739999999995</v>
+        <v>4.2769857433808525E-2</v>
+      </c>
+      <c r="B13">
+        <v>34.5794392523364</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>0.18216399999999999</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.65893409999999997</v>
+        <v>4.4806517311608875E-2</v>
+      </c>
+      <c r="B14">
+        <v>37.071651090342598</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>0.21035799999999999</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.65760090000000004</v>
+        <v>4.684317718940937E-2</v>
+      </c>
+      <c r="B15">
+        <v>40.809968847352003</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>0.244951</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.65560109999999994</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>5.0916496945010221E-2</v>
+      </c>
+      <c r="B16">
+        <v>44.236760124610505</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>0.278144</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.65260139999999989</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>5.2953156822810564E-2</v>
+      </c>
+      <c r="B17">
+        <v>47.0404984423675</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>0.314137</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.64960169999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>5.7026476578411409E-2</v>
+      </c>
+      <c r="B18">
+        <v>49.532710280373799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>0.34233200000000003</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0.64660200000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>5.9063136456211765E-2</v>
+      </c>
+      <c r="B19">
+        <v>52.024922118380005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>0.37832399999999999</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0.64326899999999998</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+        <v>6.5173116089612959E-2</v>
+      </c>
+      <c r="B20">
+        <v>54.517133956386196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>0.408918</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0.63993599999999995</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>7.1283095723014153E-2</v>
+      </c>
+      <c r="B21">
+        <v>56.386292834890902</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>0.441112</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0.63660300000000003</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>7.9429735234215842E-2</v>
+      </c>
+      <c r="B22">
+        <v>58.566978193146404</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>0.47190599999999999</v>
-      </c>
-      <c r="B23" s="2">
-        <v>0.63360329999999998</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>8.553971486761705E-2</v>
+      </c>
+      <c r="B23">
+        <v>60.124610591900293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>0.50009999999999999</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0.63060360000000004</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>9.7759674134419439E-2</v>
+      </c>
+      <c r="B24">
+        <v>62.616822429906506</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>0.530694</v>
-      </c>
-      <c r="B25" s="2">
-        <v>0.62760389999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.10794297352342148</v>
+      </c>
+      <c r="B25">
+        <v>64.485981308411198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>0.56548699999999996</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0.62393759999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.11608961303462317</v>
+      </c>
+      <c r="B26">
+        <v>65.732087227414297</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>0.60647899999999999</v>
-      </c>
-      <c r="B27" s="2">
-        <v>0.61993799999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.12627291242362523</v>
+      </c>
+      <c r="B27">
+        <v>67.289719626168193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>0.64866999999999997</v>
-      </c>
-      <c r="B28" s="2">
-        <v>0.61560509999999991</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.13849287169042762</v>
+      </c>
+      <c r="B28">
+        <v>68.535825545171306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>0.689662</v>
-      </c>
-      <c r="B29" s="2">
-        <v>0.61193879999999989</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.15478615071282983</v>
+      </c>
+      <c r="B29">
+        <v>69.470404984423595</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>0.73725300000000005</v>
-      </c>
-      <c r="B30" s="2">
-        <v>0.60727259999999994</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.17515274949083479</v>
+      </c>
+      <c r="B30">
+        <v>69.781931464174392</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>0.78724300000000003</v>
-      </c>
-      <c r="B31" s="2">
-        <v>0.60260639999999988</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.19551934826883829</v>
+      </c>
+      <c r="B31">
+        <v>69.781931464174392</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>0.83583300000000005</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0.59860679999999999</v>
+        <v>0.20977596741344132</v>
+      </c>
+      <c r="B32">
+        <v>69.470404984423595</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>0.88082400000000005</v>
-      </c>
-      <c r="B33" s="2">
-        <v>0.59460719999999989</v>
+        <v>0.22810590631364419</v>
+      </c>
+      <c r="B33">
+        <v>69.470404984423595</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>0.92561499999999997</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0.59094089999999999</v>
+        <v>0.2586558044806509</v>
+      </c>
+      <c r="B34">
+        <v>69.158878504672799</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>0.96020799999999995</v>
-      </c>
-      <c r="B35" s="2">
-        <v>0.58760789999999996</v>
+        <v>0.30957230142566117</v>
+      </c>
+      <c r="B35">
+        <v>68.847352024922102</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
+        <v>0.34215885947046842</v>
+      </c>
+      <c r="B36">
+        <v>67.9127725856697</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>0.37678207739307495</v>
+      </c>
+      <c r="B37">
+        <v>66.978193146417397</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>0.4114052953156816</v>
+      </c>
+      <c r="B38">
+        <v>66.6666666666666</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>0.4419551934826883</v>
+      </c>
+      <c r="B39">
+        <v>65.420560747663501</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>0.47454175152749412</v>
+      </c>
+      <c r="B40">
+        <v>64.485981308411198</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>0.50305498981670027</v>
+      </c>
+      <c r="B41">
+        <v>64.174454828660402</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>0.53156822810590487</v>
+      </c>
+      <c r="B42">
+        <v>63.862928348909598</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>0.56415478615071213</v>
+      </c>
+      <c r="B43">
+        <v>63.551401869158795</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>0.59266802443991828</v>
+      </c>
+      <c r="B44">
+        <v>63.239875389408098</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>0.62525458248472421</v>
+      </c>
+      <c r="B45">
+        <v>62.616822429906506</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>0.65987780040733068</v>
+      </c>
+      <c r="B46">
+        <v>62.305295950155703</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>0.69450101832993871</v>
+      </c>
+      <c r="B47">
+        <v>61.370716510903399</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>0.73523421588594573</v>
+      </c>
+      <c r="B48">
+        <v>60.436137071650997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>0.79429735234215848</v>
+      </c>
+      <c r="B49">
+        <v>60.124610591900293</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>0.82484725050916374</v>
+      </c>
+      <c r="B50">
+        <v>59.501557632398708</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>0.85743380855397111</v>
+      </c>
+      <c r="B51">
+        <v>59.190031152647904</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>0.89409368635437825</v>
+      </c>
+      <c r="B52">
+        <v>58.566978193146404</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>0.92871690427698483</v>
+      </c>
+      <c r="B53">
+        <v>58.255451713395601</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>0.96537678207739197</v>
+      </c>
+      <c r="B54">
+        <v>57.943925233644798</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55">
         <v>1</v>
       </c>
-      <c r="B36" s="2">
-        <v>0.5849415</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" s="1"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B76" s="1"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B77" s="1"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B78" s="1"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B79" s="1"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B80" s="1"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B81" s="1"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B82" s="1"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B84" s="1"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B86" s="1"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B87" s="1"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B90" s="1"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B91" s="1"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B92" s="1"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B93" s="1"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B94" s="1"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B95" s="1"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B96" s="1"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B97" s="1"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B98" s="1"/>
+      <c r="B55">
+        <v>57.943925233644798</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20040AC2-246C-4C76-A39F-5F3C71B48CC3}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1761,7 +2320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9CF4AA-6B39-4ABA-BF7A-FB938F21D187}">
   <dimension ref="A1:B32"/>
   <sheetViews>
@@ -2032,7 +2591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F4518F-E053-4336-B711-7AA8B14FF1BD}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -2093,18 +2652,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2234,6 +2793,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B262E79E-1059-4691-9D04-9A88B2733848}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31C2E850-DDF8-47DF-A688-11B6EB2C2893}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2245,14 +2812,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B262E79E-1059-4691-9D04-9A88B2733848}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>